<commit_message>
Modified example grading sheet
</commit_message>
<xml_diff>
--- a/grading.xlsx
+++ b/grading.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ylli\Documents\HEIG-VD\2025-2026\PRG1\Outils\typscript\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ylli\Repositories\FazlijaYlli@github.com\heig-grading-typscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75D6BAB-42D1-4372-9890-2A5A42B1CECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1C84119-3C26-4B18-B11D-57EF6B63D331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{B981C194-32B8-4B77-9C1C-3899EAC35078}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B981C194-32B8-4B77-9C1C-3899EAC35078}"/>
   </bookViews>
   <sheets>
     <sheet name="Grading" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,64 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ylli</author>
+  </authors>
+  <commentList>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{71FF6F92-A140-470F-9EA0-DC1C5107A30F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ylli:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not very good work. (-2 pts)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{F1ED684D-D3E6-4EA1-A363-74BEBF17D18B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ylli:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Great work !</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,7 +390,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,6 +471,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1233,11 +1304,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957BF28D-05D8-4DDC-BE7A-FBB03AC9C03E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957BF28D-05D8-4DDC-BE7A-FBB03AC9C03E}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,7 +1477,7 @@
       </c>
       <c r="F4" s="14">
         <f t="shared" ref="F4:Q4" si="0">SUM(F5:F14)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="14">
         <f t="shared" si="0"/>
@@ -1418,7 +1489,7 @@
       </c>
       <c r="I4" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="14">
         <f t="shared" si="0"/>
@@ -1521,13 +1592,13 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.11538461538461539</v>
       </c>
       <c r="E6" s="17">
         <v>0</v>
       </c>
       <c r="F6" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6" s="17">
         <v>0</v>
@@ -1536,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J6" s="17">
         <v>0</v>
@@ -2297,7 +2368,7 @@
       </c>
       <c r="D20" s="3">
         <f>AVERAGE(E20:Q20)</f>
-        <v>0</v>
+        <v>0.46153846153846156</v>
       </c>
       <c r="E20" s="23">
         <f>SUM(E5:E14)+SUM(E16:E19)</f>
@@ -2305,7 +2376,7 @@
       </c>
       <c r="F20" s="23">
         <f t="shared" ref="F20:Q20" si="5">SUM(F5:F14)+SUM(F16:F19)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G20" s="23">
         <f t="shared" si="5"/>
@@ -2317,7 +2388,7 @@
       </c>
       <c r="I20" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J20" s="23">
         <f t="shared" si="5"/>
@@ -2368,7 +2439,7 @@
       </c>
       <c r="F21" s="44">
         <f t="shared" ref="F21:Q21" si="6">1+(F20/$C$20*5)</f>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G21" s="44">
         <f t="shared" si="6"/>
@@ -2380,7 +2451,7 @@
       </c>
       <c r="I21" s="44">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="J21" s="44">
         <f t="shared" si="6"/>
@@ -2707,7 +2778,7 @@
       </c>
       <c r="F28" s="39">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G28" s="39">
         <f t="shared" si="8"/>
@@ -2719,7 +2790,7 @@
       </c>
       <c r="I28" s="39">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="J28" s="39">
         <f t="shared" si="8"/>
@@ -2782,5 +2853,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>